<commit_message>
add Romansh to docs, testdata, and templates
</commit_message>
<xml_diff>
--- a/docs/assets/templates/properties_template.xlsx
+++ b/docs/assets/templates/properties_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nusjoh00-adm/Desktop/dsp-tools/docs/assets/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6185FD1-CD01-4747-9E8D-B5F85EC1DF8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231EFDE3-83EA-C542-881D-1E5901A16A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="19520" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>name</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>gui_attributes</t>
+  </si>
+  <si>
+    <t>rm</t>
+  </si>
+  <si>
+    <t>comment_rm</t>
   </si>
 </sst>
 </file>
@@ -529,7 +535,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
@@ -540,7 +546,7 @@
     <col min="1" max="1" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -563,60 +569,66 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="L2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
     </row>
   </sheetData>

</xml_diff>